<commit_message>
correct spreadsheet typos '* 0 ' -> '* = 0', generalize severity columns in generate script
</commit_message>
<xml_diff>
--- a/specifications/ScriptRules_Fire.xlsx
+++ b/specifications/ScriptRules_Fire.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="271">
   <si>
     <t xml:space="preserve">Filename</t>
   </si>
@@ -382,7 +382,7 @@
     <t xml:space="preserve">* = 0.4</t>
   </si>
   <si>
-    <t xml:space="preserve">* 0.05</t>
+    <t xml:space="preserve">* = 0.05</t>
   </si>
   <si>
     <t xml:space="preserve">eCANOPY_TREES_UNDERSTORY_STEM_DENSITY</t>
@@ -521,9 +521,6 @@
   </si>
   <si>
     <t xml:space="preserve">* = 1 / (0.25*1.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* = 0.05</t>
   </si>
   <si>
     <t xml:space="preserve">* = (1/0.05) * 0.5</t>
@@ -912,7 +909,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -921,20 +918,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDEEBF7"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFBE5D6"/>
-        <bgColor rgb="FFDEEBF7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -968,7 +953,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -992,13 +977,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1007,7 +986,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1023,15 +1002,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1039,19 +1018,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1059,11 +1038,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1083,15 +1062,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1099,26 +1078,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Note" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in 20% - Accent1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in 20% - Accent2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFBE5D6"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -1135,8 +1112,8 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFDEEBF7"/>
+      <rgbColor rgb="FFFBE5D6"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -1186,14 +1163,14 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.9878542510121"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="258.048582995951"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="262.87044534413"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1381,15 +1358,15 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1623,12 +1600,12 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
+      <selection pane="topLeft" activeCell="J41" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="102.834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.546558704453"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1750,22 +1727,22 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G64" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H82" activeCellId="0" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="73.5910931174089"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="44.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="41.7773279352227"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="43.2753036437247"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="41.4534412955466"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="45.2024291497976"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="48.417004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="74.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="42.0971659919028"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="46.0607287449393"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="49.2753036437247"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="4" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2552,18 +2529,18 @@
         <v>164</v>
       </c>
       <c r="H35" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I35" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="J35" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>161</v>
@@ -2584,18 +2561,18 @@
         <v>164</v>
       </c>
       <c r="H36" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I36" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="J36" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>161</v>
@@ -2616,18 +2593,18 @@
         <v>164</v>
       </c>
       <c r="H37" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I37" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="J37" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>161</v>
@@ -2648,18 +2625,18 @@
         <v>164</v>
       </c>
       <c r="H38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I38" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="J38" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>161</v>
@@ -2680,18 +2657,18 @@
         <v>164</v>
       </c>
       <c r="H39" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I39" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I39" s="14" t="s">
+      <c r="J39" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J39" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>161</v>
@@ -2712,18 +2689,18 @@
         <v>164</v>
       </c>
       <c r="H40" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I40" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="J40" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B41" s="0"/>
       <c r="C41" s="0"/>
@@ -2737,7 +2714,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42" s="0"/>
       <c r="C42" s="0"/>
@@ -2751,231 +2728,231 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D43" s="0"/>
       <c r="E43" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G43" s="0"/>
       <c r="H43" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I43" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I43" s="14" t="s">
+      <c r="J43" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J43" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D44" s="0"/>
       <c r="E44" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G44" s="0"/>
       <c r="H44" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I44" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I44" s="14" t="s">
+      <c r="J44" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J44" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D45" s="0"/>
       <c r="E45" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G45" s="0"/>
       <c r="H45" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I45" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I45" s="14" t="s">
+      <c r="J45" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" s="0"/>
       <c r="E46" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G46" s="0"/>
       <c r="H46" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I46" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I46" s="14" t="s">
+      <c r="J46" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D47" s="0"/>
       <c r="E47" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G47" s="0"/>
       <c r="H47" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I47" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I47" s="14" t="s">
+      <c r="J47" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J47" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D48" s="0"/>
       <c r="E48" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G48" s="0"/>
       <c r="H48" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I48" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I48" s="14" t="s">
+      <c r="J48" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J48" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D49" s="0"/>
       <c r="E49" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G49" s="0"/>
       <c r="H49" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I49" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I49" s="14" t="s">
+      <c r="J49" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J49" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>161</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D50" s="0"/>
       <c r="E50" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G50" s="0"/>
       <c r="H50" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I50" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I50" s="14" t="s">
+      <c r="J50" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="J50" s="15" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>161</v>
@@ -2993,21 +2970,21 @@
         <v>162</v>
       </c>
       <c r="G51" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J51" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I51" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J51" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>161</v>
@@ -3025,21 +3002,21 @@
         <v>162</v>
       </c>
       <c r="G52" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J52" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J52" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>161</v>
@@ -3057,21 +3034,21 @@
         <v>162</v>
       </c>
       <c r="G53" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J53" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J53" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>161</v>
@@ -3089,21 +3066,21 @@
         <v>162</v>
       </c>
       <c r="G54" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J54" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J54" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>161</v>
@@ -3121,35 +3098,35 @@
         <v>162</v>
       </c>
       <c r="G55" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="J55" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I55" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="J55" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C56" s="0"/>
       <c r="D56" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F56" s="0"/>
       <c r="G56" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>161</v>
@@ -3159,21 +3136,21 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C57" s="0"/>
       <c r="D57" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F57" s="0"/>
       <c r="G57" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>161</v>
@@ -3183,21 +3160,21 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="0"/>
       <c r="D58" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F58" s="0"/>
       <c r="G58" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>161</v>
@@ -3207,21 +3184,21 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C59" s="0"/>
       <c r="D59" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F59" s="0"/>
       <c r="G59" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>161</v>
@@ -3231,21 +3208,21 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C60" s="0"/>
       <c r="D60" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F60" s="0"/>
       <c r="G60" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>161</v>
@@ -3255,21 +3232,21 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C61" s="0"/>
       <c r="D61" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>193</v>
       </c>
       <c r="F61" s="0"/>
       <c r="G61" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>161</v>
@@ -3279,7 +3256,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B62" s="0"/>
       <c r="C62" s="0"/>
@@ -3292,7 +3269,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B63" s="0"/>
       <c r="C63" s="0"/>
@@ -3305,7 +3282,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B64" s="0"/>
       <c r="C64" s="0"/>
@@ -3318,14 +3295,14 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C65" s="0"/>
       <c r="E65" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F65" s="0"/>
       <c r="G65" s="0"/>
@@ -3337,14 +3314,14 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C66" s="0"/>
       <c r="E66" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F66" s="0"/>
       <c r="G66" s="0"/>
@@ -3356,14 +3333,14 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C67" s="0"/>
       <c r="E67" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F67" s="0"/>
       <c r="G67" s="0"/>
@@ -3375,14 +3352,14 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C68" s="0"/>
       <c r="E68" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F68" s="0"/>
       <c r="G68" s="0"/>
@@ -3394,14 +3371,14 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C69" s="0"/>
       <c r="E69" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F69" s="0"/>
       <c r="G69" s="0"/>
@@ -3413,14 +3390,14 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C70" s="0"/>
       <c r="E70" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F70" s="0"/>
       <c r="G70" s="0"/>
@@ -3432,10 +3409,10 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C71" s="0"/>
       <c r="E71" s="5" t="s">
@@ -3451,10 +3428,10 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C72" s="0"/>
       <c r="E72" s="5" t="s">
@@ -3470,10 +3447,10 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C73" s="0"/>
       <c r="E73" s="5" t="s">
@@ -3489,7 +3466,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" s="0"/>
       <c r="C74" s="0"/>
@@ -3502,7 +3479,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B75" s="0"/>
       <c r="C75" s="0"/>
@@ -3515,7 +3492,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B76" s="0"/>
       <c r="C76" s="0"/>
@@ -3528,7 +3505,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B77" s="0"/>
       <c r="C77" s="0"/>
@@ -3541,7 +3518,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B78" s="0"/>
       <c r="C78" s="0"/>
@@ -3554,7 +3531,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B79" s="0"/>
       <c r="C79" s="0"/>
@@ -3567,7 +3544,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B80" s="0"/>
       <c r="C80" s="0"/>
@@ -3580,13 +3557,13 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C81" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C81" s="14" t="s">
-        <v>220</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>96</v>
@@ -3595,27 +3572,27 @@
         <v>101</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I81" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J81" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>96</v>
@@ -3624,21 +3601,21 @@
         <v>101</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H82" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I82" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J82" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B83" s="0"/>
       <c r="C83" s="14"/>
@@ -3651,13 +3628,13 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>96</v>
@@ -3666,27 +3643,27 @@
         <v>101</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I84" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>96</v>
@@ -3695,21 +3672,21 @@
         <v>101</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I85" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J85" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B86" s="0"/>
       <c r="C86" s="14"/>
@@ -3722,13 +3699,13 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>96</v>
@@ -3737,27 +3714,27 @@
         <v>101</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I87" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>96</v>
@@ -3766,21 +3743,21 @@
         <v>101</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H88" s="5" t="s">
         <v>118</v>
       </c>
       <c r="I88" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J88" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B89" s="0"/>
       <c r="C89" s="14"/>
@@ -3790,13 +3767,13 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>96</v>
@@ -3807,13 +3784,13 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>96</v>
@@ -3824,7 +3801,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B92" s="0"/>
       <c r="C92" s="14"/>
@@ -3833,13 +3810,13 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>96</v>
@@ -3850,13 +3827,13 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>96</v>
@@ -3867,7 +3844,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B95" s="0"/>
       <c r="C95" s="14"/>
@@ -3876,13 +3853,13 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>96</v>
@@ -3893,13 +3870,13 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>96</v>
@@ -3910,13 +3887,13 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>96</v>
@@ -3927,7 +3904,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B99" s="0"/>
       <c r="C99" s="14"/>
@@ -3936,13 +3913,13 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>96</v>
@@ -3953,13 +3930,13 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>96</v>
@@ -3970,13 +3947,13 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>96</v>
@@ -3987,7 +3964,7 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -4009,12 +3986,12 @@
   <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="103.368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="105.19028340081"/>
     <col collapsed="false" hidden="false" max="6" min="2" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="13" min="9" style="0" width="9.10526315789474"/>
@@ -4023,7 +4000,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>3</v>
@@ -4883,7 +4860,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>21.6</v>
@@ -4927,7 +4904,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>85</v>
@@ -4971,12 +4948,12 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0.3</v>
@@ -4999,7 +4976,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1.2</v>
@@ -5022,7 +4999,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>95</v>
@@ -5045,12 +5022,12 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0.9</v>
@@ -5094,7 +5071,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0.1</v>
@@ -5138,7 +5115,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0.7</v>
@@ -5182,7 +5159,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>95</v>
@@ -5226,7 +5203,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0.9</v>
@@ -5249,7 +5226,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0.1</v>
@@ -5272,7 +5249,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0.2</v>
@@ -5295,7 +5272,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>85</v>
@@ -5318,7 +5295,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>4</v>
@@ -5356,7 +5333,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>70</v>
@@ -5394,7 +5371,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>2</v>
@@ -5432,7 +5409,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1.5</v>
@@ -5470,7 +5447,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -5508,7 +5485,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>6</v>
@@ -5546,7 +5523,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>12</v>
@@ -5584,7 +5561,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -5622,7 +5599,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -5648,7 +5625,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>11</v>
@@ -5674,7 +5651,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -5700,7 +5677,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>9.6</v>
@@ -5714,7 +5691,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0.4</v>
@@ -5728,7 +5705,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>115</v>
@@ -5742,7 +5719,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>9.6</v>
@@ -5765,7 +5742,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0.4</v>
@@ -5788,7 +5765,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>115</v>
@@ -5811,22 +5788,22 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0.078119</v>
@@ -5873,7 +5850,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -5920,7 +5897,7 @@
     </row>
     <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0</v>
@@ -5967,7 +5944,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F73" s="0" t="n">
         <v>90</v>
@@ -5984,7 +5961,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>100</v>
@@ -6004,7 +5981,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>100</v>
@@ -6027,7 +6004,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B76" s="2" t="n">
         <v>50</v>
@@ -6053,7 +6030,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B77" s="2" t="n">
         <v>50</v>
@@ -6073,7 +6050,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G78" s="0" t="n">
         <v>60</v>
@@ -6081,7 +6058,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M79" s="0" t="n">
         <v>5</v>
@@ -6089,7 +6066,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>2</v>
@@ -6097,7 +6074,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>5</v>
@@ -6105,12 +6082,12 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>0.2</v>
@@ -6157,7 +6134,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>70</v>
@@ -6204,12 +6181,12 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>2.5</v>
@@ -6226,7 +6203,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>80</v>
@@ -6243,12 +6220,12 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>0.2</v>
@@ -6265,7 +6242,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>60</v>
@@ -6282,12 +6259,12 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>0.5</v>
@@ -6331,7 +6308,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>70</v>
@@ -6375,12 +6352,12 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I95" s="0" t="n">
         <v>2</v>
@@ -6397,7 +6374,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I96" s="0" t="n">
         <v>2.55</v>
@@ -6414,7 +6391,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I97" s="0" t="n">
         <v>0.5</v>
@@ -6431,12 +6408,12 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>18</v>
@@ -6444,7 +6421,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E100" s="0" t="n">
         <v>1</v>
@@ -6452,7 +6429,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E101" s="0" t="n">
         <v>5</v>
@@ -6460,7 +6437,7 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -6482,16 +6459,16 @@
   <dimension ref="1:103"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B103" activeCellId="0" sqref="B103"/>
+      <selection pane="topLeft" activeCell="B103" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="73.5910931174089"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="74.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="28.9230769230769"/>
     <col collapsed="false" hidden="true" max="4" min="4" style="6" width="0"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="41.7773279352227"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="42.4210526315789"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="19" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="20" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="21" width="9.10526315789474"/>
@@ -7547,17 +7524,17 @@
     </row>
     <row r="2" s="23" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>252</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>3</v>
@@ -10757,7 +10734,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" s="5" t="n">
         <v>0.5</v>
@@ -10862,7 +10839,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" s="5" t="n">
         <v>0.5</v>
@@ -10967,7 +10944,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B38" s="5" t="n">
         <v>0.5</v>
@@ -11006,7 +10983,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B39" s="5" t="n">
         <v>0.5</v>
@@ -11105,7 +11082,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="5" t="n">
         <v>0.5</v>
@@ -11204,7 +11181,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B41" s="5" t="n">
         <v>0.5</v>
@@ -11303,7 +11280,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42" s="5" t="n">
         <v>0.5</v>
@@ -11342,13 +11319,13 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B43" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="0"/>
@@ -11443,13 +11420,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B44" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="0"/>
@@ -11544,13 +11521,13 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B45" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="0"/>
@@ -11645,13 +11622,13 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B46" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="0"/>
@@ -11746,13 +11723,13 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B47" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="0"/>
@@ -11845,13 +11822,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B48" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D48" s="14"/>
       <c r="E48" s="0"/>
@@ -11944,13 +11921,13 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B49" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D49" s="14"/>
       <c r="E49" s="0"/>
@@ -12043,13 +12020,13 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B50" s="5" t="n">
         <v>0.5</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="0"/>
@@ -12142,7 +12119,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B51" s="5" t="n">
         <v>0.5</v>
@@ -12245,7 +12222,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B52" s="5" t="n">
         <v>0.5</v>
@@ -12348,7 +12325,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B53" s="5" t="n">
         <v>0.5</v>
@@ -12451,7 +12428,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B54" s="5" t="n">
         <v>0.5</v>
@@ -12554,7 +12531,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B55" s="5" t="n">
         <v>0.5</v>
@@ -12657,7 +12634,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B56" s="5" t="n">
         <v>0.9</v>
@@ -12665,7 +12642,7 @@
       <c r="C56" s="0"/>
       <c r="D56" s="0"/>
       <c r="E56" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F56" s="19" t="n">
         <v>6</v>
@@ -12758,7 +12735,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B57" s="5" t="n">
         <v>0.9</v>
@@ -12766,7 +12743,7 @@
       <c r="C57" s="0"/>
       <c r="D57" s="0"/>
       <c r="E57" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F57" s="19" t="n">
         <v>12</v>
@@ -12859,7 +12836,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B58" s="5" t="n">
         <v>0.9</v>
@@ -12867,7 +12844,7 @@
       <c r="C58" s="0"/>
       <c r="D58" s="0"/>
       <c r="E58" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F58" s="19" t="n">
         <v>0</v>
@@ -12960,7 +12937,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B59" s="5" t="n">
         <v>0.9</v>
@@ -12968,7 +12945,7 @@
       <c r="C59" s="0"/>
       <c r="D59" s="0"/>
       <c r="E59" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F59" s="19" t="n">
         <v>5</v>
@@ -13057,7 +13034,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B60" s="5" t="n">
         <v>0.9</v>
@@ -13065,7 +13042,7 @@
       <c r="C60" s="0"/>
       <c r="D60" s="0"/>
       <c r="E60" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F60" s="19" t="n">
         <v>11</v>
@@ -13154,7 +13131,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B61" s="5" t="n">
         <v>0.9</v>
@@ -13162,7 +13139,7 @@
       <c r="C61" s="0"/>
       <c r="D61" s="0"/>
       <c r="E61" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F61" s="19" t="n">
         <v>0</v>
@@ -13251,7 +13228,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="0"/>
@@ -13341,7 +13318,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="0"/>
@@ -13431,7 +13408,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="0"/>
@@ -13521,7 +13498,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B65" s="5" t="n">
         <v>0.9</v>
@@ -13617,7 +13594,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B66" s="5" t="n">
         <v>0.9</v>
@@ -13713,7 +13690,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B67" s="5" t="n">
         <v>0.9</v>
@@ -13809,7 +13786,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B68" s="5" t="n">
         <v>0.9</v>
@@ -13897,7 +13874,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B69" s="5" t="n">
         <v>0.9</v>
@@ -13985,7 +13962,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B70" s="5" t="n">
         <v>0.9</v>
@@ -14073,7 +14050,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B71" s="5" t="n">
         <v>0.75</v>
@@ -14173,7 +14150,7 @@
     </row>
     <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B72" s="5" t="n">
         <v>0.75</v>
@@ -14273,7 +14250,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B73" s="5" t="n">
         <v>0.75</v>
@@ -14373,7 +14350,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="0"/>
@@ -14461,7 +14438,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B75" s="5"/>
       <c r="C75" s="0"/>
@@ -14549,7 +14526,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B76" s="5"/>
       <c r="C76" s="0"/>
@@ -14637,7 +14614,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="0"/>
@@ -14729,7 +14706,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="0"/>
@@ -14819,7 +14796,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B79" s="5"/>
       <c r="C79" s="0"/>
@@ -14907,7 +14884,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="0"/>
@@ -14993,13 +14970,13 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B81" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D81" s="14"/>
       <c r="F81" s="0"/>
@@ -15085,13 +15062,13 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B82" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D82" s="14"/>
       <c r="F82" s="0"/>
@@ -15177,13 +15154,13 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B83" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D83" s="14"/>
       <c r="F83" s="0"/>
@@ -15213,13 +15190,13 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B84" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D84" s="14"/>
       <c r="F84" s="19" t="n">
@@ -15315,13 +15292,13 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B85" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D85" s="14"/>
       <c r="F85" s="19" t="n">
@@ -15417,13 +15394,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B86" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D86" s="14"/>
       <c r="F86" s="0"/>
@@ -15453,13 +15430,13 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B87" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D87" s="14"/>
       <c r="F87" s="0"/>
@@ -15547,13 +15524,13 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B88" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D88" s="14"/>
       <c r="F88" s="0"/>
@@ -15641,13 +15618,13 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B89" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D89" s="14"/>
       <c r="F89" s="0"/>
@@ -15677,13 +15654,13 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B90" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D90" s="14"/>
       <c r="F90" s="0"/>
@@ -15771,13 +15748,13 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B91" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D91" s="14"/>
       <c r="F91" s="0"/>
@@ -15865,13 +15842,13 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B92" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D92" s="14"/>
       <c r="F92" s="0"/>
@@ -15901,13 +15878,13 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B93" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D93" s="14"/>
       <c r="F93" s="19" t="n">
@@ -16003,13 +15980,13 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B94" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D94" s="14"/>
       <c r="F94" s="19" t="n">
@@ -16105,13 +16082,13 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B95" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D95" s="14"/>
       <c r="G95" s="0"/>
@@ -16136,13 +16113,13 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B96" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D96" s="14"/>
       <c r="G96" s="20" t="n">
@@ -16221,13 +16198,13 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B97" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D97" s="14"/>
       <c r="G97" s="20" t="n">
@@ -16306,13 +16283,13 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B98" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D98" s="14"/>
       <c r="G98" s="20" t="n">
@@ -16391,13 +16368,13 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B99" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D99" s="14"/>
       <c r="G99" s="0"/>
@@ -16422,13 +16399,13 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B100" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D100" s="14"/>
       <c r="G100" s="20" t="n">
@@ -16509,13 +16486,13 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B101" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D101" s="14"/>
       <c r="G101" s="20" t="n">
@@ -16596,13 +16573,13 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B102" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D102" s="14"/>
       <c r="G102" s="20" t="n">
@@ -16683,13 +16660,13 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B103" s="5" t="n">
         <v>0.75</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -16711,100 +16688,100 @@
   <dimension ref="A1:Y102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="73.5910931174089"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="74.8744939271255"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>255</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>256</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>258</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>259</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>261</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>262</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>24</v>
       </c>
       <c r="O1" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="P1" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>264</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>265</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>27</v>
       </c>
       <c r="S1" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="T1" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>267</v>
-      </c>
-      <c r="U1" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="V1" s="0" t="s">
         <v>42</v>
       </c>
       <c r="W1" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="X1" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="Y1" s="0" t="s">
         <v>270</v>
-      </c>
-      <c r="Y1" s="0" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19014,7 +18991,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>21.6</v>
@@ -19091,7 +19068,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>85</v>
@@ -19168,12 +19145,12 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0.3</v>
@@ -19241,7 +19218,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1.2</v>
@@ -19309,7 +19286,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>95</v>
@@ -19377,12 +19354,12 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0.9</v>
@@ -19456,7 +19433,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0.1</v>
@@ -19530,7 +19507,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0.7</v>
@@ -19604,7 +19581,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>95</v>
@@ -19678,7 +19655,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0.9</v>
@@ -19749,7 +19726,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0.1</v>
@@ -19820,7 +19797,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0.2</v>
@@ -19891,7 +19868,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>85</v>
@@ -19962,7 +19939,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>4</v>
@@ -20036,7 +20013,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>70</v>
@@ -20110,7 +20087,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>2</v>
@@ -20184,7 +20161,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1.5</v>
@@ -20258,7 +20235,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -20332,7 +20309,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>6</v>
@@ -20406,7 +20383,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>12</v>
@@ -20480,7 +20457,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -20554,7 +20531,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -20622,7 +20599,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>11</v>
@@ -20690,7 +20667,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>
@@ -20758,7 +20735,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>9.6</v>
@@ -20823,7 +20800,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0.4</v>
@@ -20888,7 +20865,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>115</v>
@@ -20953,7 +20930,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>9.6</v>
@@ -21024,7 +21001,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>0.4</v>
@@ -21095,7 +21072,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>115</v>
@@ -21166,7 +21143,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>0</v>
@@ -21225,7 +21202,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>0</v>
@@ -21284,7 +21261,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>0</v>
@@ -21343,7 +21320,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0.078119</v>
@@ -21420,7 +21397,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0</v>
@@ -21497,7 +21474,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>0</v>
@@ -21574,7 +21551,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>0</v>
@@ -21636,7 +21613,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>0</v>
@@ -21698,7 +21675,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>0</v>
@@ -21760,7 +21737,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>50</v>
@@ -21828,7 +21805,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>50</v>
@@ -21893,7 +21870,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>0</v>
@@ -21955,7 +21932,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>0</v>
@@ -22014,7 +21991,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>0</v>
@@ -22076,7 +22053,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>0</v>
@@ -22138,12 +22115,12 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>0.2</v>
@@ -22220,7 +22197,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>70</v>
@@ -22297,12 +22274,12 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>0</v>
@@ -22367,7 +22344,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>0</v>
@@ -22432,12 +22409,12 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>0</v>
@@ -22502,7 +22479,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>0</v>
@@ -22567,12 +22544,12 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>0.5</v>
@@ -22649,7 +22626,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>70</v>
@@ -22726,12 +22703,12 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>0</v>
@@ -22790,7 +22767,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>0</v>
@@ -22849,7 +22826,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>0</v>
@@ -22908,12 +22885,12 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>0</v>
@@ -22975,7 +22952,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C100" s="0" t="n">
         <v>0</v>
@@ -23037,7 +23014,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>0</v>
@@ -23099,7 +23076,7 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change to reflect new filenaming strategy
</commit_message>
<xml_diff>
--- a/specifications/ScriptRules_Fire.xlsx
+++ b/specifications/ScriptRules_Fire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="1" state="visible" r:id="rId2"/>
@@ -1163,14 +1163,14 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 B27"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0566801619433"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="262.87044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="0.00404858299595142"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1358,15 +1358,15 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2429149797571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1600,12 +1600,12 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J41" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 J41"/>
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.546558704453"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.51012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1727,22 +1727,22 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G64" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H82" activeCellId="0" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G64" colorId="64" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H82" activeCellId="0" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="74.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="45.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="42.4210526315789"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="43.919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="42.0971659919028"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="46.0607287449393"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="75.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="42.7408906882591"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="44.2388663967611"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="46.4898785425101"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="49.5951417004049"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="4" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3986,12 +3986,12 @@
   <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="105.19028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="106.153846153846"/>
     <col collapsed="false" hidden="false" max="6" min="2" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="13" min="9" style="0" width="9.10526315789474"/>
@@ -6459,16 +6459,16 @@
   <dimension ref="1:103"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B103" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 B103"/>
+      <selection pane="topLeft" activeCell="B103" activeCellId="0" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="74.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="75.5182186234818"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="18" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="29.1376518218623"/>
     <col collapsed="false" hidden="true" max="4" min="4" style="6" width="0"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="42.7408906882591"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="19" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="20" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="21" width="9.10526315789474"/>
@@ -16687,23 +16687,23 @@
   </sheetPr>
   <dimension ref="A1:Y102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="7" sqref="H82 H84:H85 H87:H88 H90:H91 H93:H94 H96:H98 H100:H102 D22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="74.8744939271255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="84.6720647773279"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -20309,7 +20309,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>244</v>
+        <v>190</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>6</v>
@@ -20383,7 +20383,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>12</v>
@@ -20457,7 +20457,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>246</v>
+        <v>195</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -20531,7 +20531,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>5</v>
@@ -20599,7 +20599,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>11</v>
@@ -20667,7 +20667,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>249</v>
+        <v>198</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Corrected percent live shrub spec line
</commit_message>
<xml_diff>
--- a/specifications/ScriptRules_Fire.xlsx
+++ b/specifications/ScriptRules_Fire.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="HighExpected" sheetId="8" r:id="rId8"/>
     <sheet name="Expected" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="313">
   <si>
     <t>Filename</t>
   </si>
@@ -2085,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK94"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3036,12 +3036,24 @@
       <c r="A40" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40" s="15"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
+      <c r="B40" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="H40" s="5" t="s">
         <v>118</v>
       </c>
@@ -6698,16 +6710,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView topLeftCell="P2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.5703125"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="9.140625" style="21"/>
     <col min="11" max="11" width="9.140625" style="20"/>
@@ -24227,7 +24239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A47" activePane="bottomLeft"/>
       <selection activeCell="AB2" sqref="AB1:AB1048576"/>
       <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
@@ -27382,7 +27394,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H35" s="35">
-        <f t="shared" ref="H35:H59" si="34">$D35*G35</f>
+        <f t="shared" ref="H35:H53" si="34">$D35*G35</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I35" s="26">
@@ -29331,7 +29343,7 @@
         <v>3</v>
       </c>
       <c r="H54" s="35">
-        <f>G54</f>
+        <f t="shared" ref="H54:H59" si="51">G54</f>
         <v>3</v>
       </c>
       <c r="I54" s="26">
@@ -29342,11 +29354,11 @@
         <v>0</v>
       </c>
       <c r="K54" s="28">
-        <f t="shared" ref="K54:L78" si="51">J54</f>
+        <f t="shared" ref="K54:L78" si="52">J54</f>
         <v>0</v>
       </c>
       <c r="L54" s="35">
-        <f>K54</f>
+        <f t="shared" ref="L54:L59" si="53">K54</f>
         <v>0</v>
       </c>
       <c r="N54" s="27">
@@ -29354,11 +29366,11 @@
         <v>0</v>
       </c>
       <c r="O54" s="28">
-        <f t="shared" ref="O54:P78" si="52">N54</f>
+        <f t="shared" ref="O54:P78" si="54">N54</f>
         <v>0</v>
       </c>
       <c r="P54" s="35">
-        <f>O54</f>
+        <f t="shared" ref="P54:P59" si="55">O54</f>
         <v>0</v>
       </c>
       <c r="Q54" s="26">
@@ -29369,11 +29381,11 @@
         <v>0.5</v>
       </c>
       <c r="S54" s="28">
-        <f t="shared" ref="S54:T78" si="53">R54</f>
+        <f t="shared" ref="S54:T78" si="56">R54</f>
         <v>0.5</v>
       </c>
       <c r="T54" s="35">
-        <f>S54</f>
+        <f t="shared" ref="T54:T59" si="57">S54</f>
         <v>0.5</v>
       </c>
       <c r="U54" s="26">
@@ -29384,11 +29396,11 @@
         <v>0.6</v>
       </c>
       <c r="W54" s="28">
-        <f t="shared" ref="W54:X78" si="54">V54</f>
+        <f t="shared" ref="W54:X78" si="58">V54</f>
         <v>0.6</v>
       </c>
       <c r="X54" s="35">
-        <f>W54</f>
+        <f t="shared" ref="X54:X59" si="59">W54</f>
         <v>0.6</v>
       </c>
       <c r="Y54" s="26">
@@ -29399,11 +29411,11 @@
         <v>0.25</v>
       </c>
       <c r="AA54" s="28">
-        <f t="shared" ref="AA54:AB78" si="55">Z54</f>
+        <f t="shared" ref="AA54:AB78" si="60">Z54</f>
         <v>0.25</v>
       </c>
       <c r="AB54" s="35">
-        <f>AA54</f>
+        <f t="shared" ref="AB54:AB59" si="61">AA54</f>
         <v>0.25</v>
       </c>
     </row>
@@ -29429,7 +29441,7 @@
         <v>6</v>
       </c>
       <c r="H55" s="35">
-        <f>G55</f>
+        <f t="shared" si="51"/>
         <v>6</v>
       </c>
       <c r="I55" s="26">
@@ -29440,11 +29452,11 @@
         <v>0</v>
       </c>
       <c r="K55" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L55" s="35">
-        <f>K55</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N55" s="27">
@@ -29452,11 +29464,11 @@
         <v>0</v>
       </c>
       <c r="O55" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P55" s="35">
-        <f>O55</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="Q55" s="26">
@@ -29467,11 +29479,11 @@
         <v>0</v>
       </c>
       <c r="S55" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="T55" s="35">
-        <f>S55</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="U55" s="26">
@@ -29482,11 +29494,11 @@
         <v>0.25</v>
       </c>
       <c r="W55" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.25</v>
       </c>
       <c r="X55" s="35">
-        <f>W55</f>
+        <f t="shared" si="59"/>
         <v>0.25</v>
       </c>
       <c r="Y55" s="26">
@@ -29497,11 +29509,11 @@
         <v>0</v>
       </c>
       <c r="AA55" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB55" s="35">
-        <f>AA55</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
@@ -29527,7 +29539,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="35">
-        <f>G56</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="I56" s="26">
@@ -29538,11 +29550,11 @@
         <v>0</v>
       </c>
       <c r="K56" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L56" s="35">
-        <f>K56</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N56" s="27">
@@ -29550,11 +29562,11 @@
         <v>0</v>
       </c>
       <c r="O56" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P56" s="35">
-        <f>O56</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="Q56" s="26">
@@ -29565,11 +29577,11 @@
         <v>0</v>
       </c>
       <c r="S56" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="T56" s="35">
-        <f>S56</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="U56" s="26">
@@ -29580,11 +29592,11 @@
         <v>0.25</v>
       </c>
       <c r="W56" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.25</v>
       </c>
       <c r="X56" s="35">
-        <f>W56</f>
+        <f t="shared" si="59"/>
         <v>0.25</v>
       </c>
       <c r="Y56" s="26">
@@ -29595,11 +29607,11 @@
         <v>0</v>
       </c>
       <c r="AA56" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB56" s="35">
-        <f>AA56</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
@@ -29625,7 +29637,7 @@
         <v>2.5</v>
       </c>
       <c r="H57" s="35">
-        <f>G57</f>
+        <f t="shared" si="51"/>
         <v>2.5</v>
       </c>
       <c r="J57" s="27">
@@ -29633,11 +29645,11 @@
         <v>0</v>
       </c>
       <c r="K57" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L57" s="35">
-        <f>K57</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N57" s="27">
@@ -29645,11 +29657,11 @@
         <v>0</v>
       </c>
       <c r="O57" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P57" s="35">
-        <f>O57</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="Q57" s="26">
@@ -29660,11 +29672,11 @@
         <v>0.25</v>
       </c>
       <c r="S57" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0.25</v>
       </c>
       <c r="T57" s="35">
-        <f>S57</f>
+        <f t="shared" si="57"/>
         <v>0.25</v>
       </c>
       <c r="U57" s="26">
@@ -29675,11 +29687,11 @@
         <v>0.375</v>
       </c>
       <c r="W57" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.375</v>
       </c>
       <c r="X57" s="35">
-        <f>W57</f>
+        <f t="shared" si="59"/>
         <v>0.375</v>
       </c>
       <c r="Z57" s="27">
@@ -29687,11 +29699,11 @@
         <v>0</v>
       </c>
       <c r="AA57" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB57" s="35">
-        <f>AA57</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
@@ -29717,7 +29729,7 @@
         <v>5.5</v>
       </c>
       <c r="H58" s="35">
-        <f>G58</f>
+        <f t="shared" si="51"/>
         <v>5.5</v>
       </c>
       <c r="J58" s="27">
@@ -29725,11 +29737,11 @@
         <v>0</v>
       </c>
       <c r="K58" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L58" s="35">
-        <f>K58</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N58" s="27">
@@ -29737,11 +29749,11 @@
         <v>0</v>
       </c>
       <c r="O58" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P58" s="35">
-        <f>O58</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="Q58" s="26">
@@ -29752,11 +29764,11 @@
         <v>0</v>
       </c>
       <c r="S58" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="T58" s="35">
-        <f>S58</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="U58" s="26">
@@ -29767,11 +29779,11 @@
         <v>0.15</v>
       </c>
       <c r="W58" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.15</v>
       </c>
       <c r="X58" s="35">
-        <f>W58</f>
+        <f t="shared" si="59"/>
         <v>0.15</v>
       </c>
       <c r="Z58" s="27">
@@ -29779,11 +29791,11 @@
         <v>0</v>
       </c>
       <c r="AA58" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB58" s="35">
-        <f>AA58</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
@@ -29809,7 +29821,7 @@
         <v>0</v>
       </c>
       <c r="H59" s="35">
-        <f>G59</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="J59" s="27">
@@ -29817,11 +29829,11 @@
         <v>0</v>
       </c>
       <c r="K59" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L59" s="35">
-        <f>K59</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N59" s="27">
@@ -29829,11 +29841,11 @@
         <v>0</v>
       </c>
       <c r="O59" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P59" s="35">
-        <f>O59</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="Q59" s="26">
@@ -29844,11 +29856,11 @@
         <v>0</v>
       </c>
       <c r="S59" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="T59" s="35">
-        <f>S59</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="U59" s="26">
@@ -29859,11 +29871,11 @@
         <v>0</v>
       </c>
       <c r="W59" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X59" s="35">
-        <f>W59</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="Z59" s="27">
@@ -29871,11 +29883,11 @@
         <v>0</v>
       </c>
       <c r="AA59" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB59" s="35">
-        <f>AA59</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
@@ -29899,7 +29911,7 @@
         <v>9.6</v>
       </c>
       <c r="H60" s="21">
-        <f t="shared" ref="H60:H78" si="56">G60</f>
+        <f t="shared" ref="H60:H78" si="62">G60</f>
         <v>9.6</v>
       </c>
       <c r="J60" s="27">
@@ -29907,11 +29919,11 @@
         <v>0</v>
       </c>
       <c r="K60" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L60" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N60" s="27">
@@ -29919,11 +29931,11 @@
         <v>0</v>
       </c>
       <c r="O60" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P60" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q60" s="26">
@@ -29934,11 +29946,11 @@
         <v>3.5</v>
       </c>
       <c r="S60" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>3.5</v>
       </c>
       <c r="T60" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>3.5</v>
       </c>
       <c r="V60" s="27">
@@ -29946,11 +29958,11 @@
         <v>0</v>
       </c>
       <c r="W60" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X60" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Z60" s="27">
@@ -29958,11 +29970,11 @@
         <v>0</v>
       </c>
       <c r="AA60" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB60" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -29986,7 +29998,7 @@
         <v>0.4</v>
       </c>
       <c r="H61" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>0.4</v>
       </c>
       <c r="J61" s="27">
@@ -29994,11 +30006,11 @@
         <v>0</v>
       </c>
       <c r="K61" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L61" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N61" s="27">
@@ -30006,11 +30018,11 @@
         <v>0</v>
       </c>
       <c r="O61" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P61" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q61" s="26">
@@ -30021,11 +30033,11 @@
         <v>2</v>
       </c>
       <c r="S61" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>2</v>
       </c>
       <c r="T61" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>2</v>
       </c>
       <c r="V61" s="27">
@@ -30033,11 +30045,11 @@
         <v>0</v>
       </c>
       <c r="W61" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X61" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Z61" s="27">
@@ -30045,11 +30057,11 @@
         <v>0</v>
       </c>
       <c r="AA61" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB61" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30073,7 +30085,7 @@
         <v>115</v>
       </c>
       <c r="H62" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>115</v>
       </c>
       <c r="J62" s="27">
@@ -30081,11 +30093,11 @@
         <v>0</v>
       </c>
       <c r="K62" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L62" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N62" s="27">
@@ -30093,11 +30105,11 @@
         <v>0</v>
       </c>
       <c r="O62" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P62" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q62" s="26">
@@ -30108,11 +30120,11 @@
         <v>50</v>
       </c>
       <c r="S62" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>50</v>
       </c>
       <c r="T62" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>50</v>
       </c>
       <c r="V62" s="27">
@@ -30120,11 +30132,11 @@
         <v>0</v>
       </c>
       <c r="W62" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X62" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Z62" s="27">
@@ -30132,11 +30144,11 @@
         <v>0</v>
       </c>
       <c r="AA62" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB62" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30154,7 +30166,7 @@
         <v>9.6</v>
       </c>
       <c r="F63" s="27">
-        <f t="shared" ref="F63:F71" si="57">$B63*E63</f>
+        <f t="shared" ref="F63:F71" si="63">$B63*E63</f>
         <v>4.8</v>
       </c>
       <c r="G63" s="28">
@@ -30162,76 +30174,76 @@
         <v>4.8</v>
       </c>
       <c r="H63" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>4.8</v>
       </c>
       <c r="J63" s="27">
-        <f t="shared" ref="J63:J71" si="58">$B63*I63</f>
+        <f t="shared" ref="J63:J71" si="64">$B63*I63</f>
         <v>0</v>
       </c>
       <c r="K63" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L63" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N63" s="27">
-        <f t="shared" ref="N63:N71" si="59">$B63*M63</f>
+        <f t="shared" ref="N63:N71" si="65">$B63*M63</f>
         <v>0</v>
       </c>
       <c r="O63" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P63" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q63" s="26">
         <v>3.5</v>
       </c>
       <c r="R63" s="27">
-        <f t="shared" ref="R63:R71" si="60">$B63*Q63</f>
+        <f t="shared" ref="R63:R71" si="66">$B63*Q63</f>
         <v>1.75</v>
       </c>
       <c r="S63" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>1.75</v>
       </c>
       <c r="T63" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>1.75</v>
       </c>
       <c r="U63" s="26">
         <v>10</v>
       </c>
       <c r="V63" s="27">
-        <f t="shared" ref="V63:V71" si="61">$B63*U63</f>
+        <f t="shared" ref="V63:V71" si="67">$B63*U63</f>
         <v>5</v>
       </c>
       <c r="W63" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>5</v>
       </c>
       <c r="X63" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>5</v>
       </c>
       <c r="Y63" s="26">
         <v>10</v>
       </c>
       <c r="Z63" s="27">
-        <f t="shared" ref="Z63:Z71" si="62">$B63*Y63</f>
+        <f t="shared" ref="Z63:Z71" si="68">$B63*Y63</f>
         <v>5</v>
       </c>
       <c r="AA63" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>5</v>
       </c>
       <c r="AB63" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>5</v>
       </c>
     </row>
@@ -30249,7 +30261,7 @@
         <v>0.4</v>
       </c>
       <c r="F64" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>0.2</v>
       </c>
       <c r="G64" s="28">
@@ -30257,76 +30269,76 @@
         <v>0.2</v>
       </c>
       <c r="H64" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>0.2</v>
       </c>
       <c r="J64" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="K64" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L64" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N64" s="27">
-        <f t="shared" si="59"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="O64" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P64" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q64" s="26">
         <v>2</v>
       </c>
       <c r="R64" s="27">
-        <f t="shared" si="60"/>
+        <f t="shared" si="66"/>
         <v>1</v>
       </c>
       <c r="S64" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>1</v>
       </c>
       <c r="T64" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>1</v>
       </c>
       <c r="U64" s="26">
         <v>1</v>
       </c>
       <c r="V64" s="27">
-        <f t="shared" si="61"/>
+        <f t="shared" si="67"/>
         <v>0.5</v>
       </c>
       <c r="W64" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.5</v>
       </c>
       <c r="X64" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.5</v>
       </c>
       <c r="Y64" s="26">
         <v>1</v>
       </c>
       <c r="Z64" s="27">
-        <f t="shared" si="62"/>
+        <f t="shared" si="68"/>
         <v>0.5</v>
       </c>
       <c r="AA64" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0.5</v>
       </c>
       <c r="AB64" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0.5</v>
       </c>
     </row>
@@ -30344,7 +30356,7 @@
         <v>115</v>
       </c>
       <c r="F65" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>57.5</v>
       </c>
       <c r="G65" s="28">
@@ -30352,76 +30364,76 @@
         <v>57.5</v>
       </c>
       <c r="H65" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>57.5</v>
       </c>
       <c r="J65" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="K65" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L65" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N65" s="27">
-        <f t="shared" si="59"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="O65" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P65" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q65" s="26">
         <v>50</v>
       </c>
       <c r="R65" s="27">
-        <f t="shared" si="60"/>
+        <f t="shared" si="66"/>
         <v>25</v>
       </c>
       <c r="S65" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>25</v>
       </c>
       <c r="T65" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>25</v>
       </c>
       <c r="U65" s="26">
         <v>5</v>
       </c>
       <c r="V65" s="27">
-        <f t="shared" si="61"/>
+        <f t="shared" si="67"/>
         <v>2.5</v>
       </c>
       <c r="W65" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>2.5</v>
       </c>
       <c r="X65" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>2.5</v>
       </c>
       <c r="Y65" s="26">
         <v>3</v>
       </c>
       <c r="Z65" s="27">
-        <f t="shared" si="62"/>
+        <f t="shared" si="68"/>
         <v>1.5</v>
       </c>
       <c r="AA65" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>1.5</v>
       </c>
       <c r="AB65" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>1.5</v>
       </c>
     </row>
@@ -30436,7 +30448,7 @@
       <c r="C66" s="32"/>
       <c r="D66" s="33"/>
       <c r="F66" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G66" s="28">
@@ -30444,67 +30456,67 @@
         <v>0</v>
       </c>
       <c r="H66" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="J66" s="27">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L66" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="N66" s="27">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="O66" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P66" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R66" s="27">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="S66" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="J66" s="27">
+      <c r="T66" s="21">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="V66" s="27">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="W66" s="28">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="K66" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L66" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="N66" s="27">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="O66" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P66" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R66" s="27">
+      <c r="X66" s="21">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="Z66" s="27">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="AA66" s="28">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="S66" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="T66" s="21">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="V66" s="27">
-        <f t="shared" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="W66" s="28">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="X66" s="21">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="Z66" s="27">
-        <f t="shared" si="62"/>
-        <v>0</v>
-      </c>
-      <c r="AA66" s="28">
-        <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
       <c r="AB66" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30519,7 +30531,7 @@
       <c r="C67" s="32"/>
       <c r="D67" s="33"/>
       <c r="F67" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G67" s="28">
@@ -30527,67 +30539,67 @@
         <v>0</v>
       </c>
       <c r="H67" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="27">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="K67" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L67" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="N67" s="27">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="O67" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P67" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R67" s="27">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="S67" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="J67" s="27">
+      <c r="T67" s="21">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="V67" s="27">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="W67" s="28">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="K67" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L67" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="N67" s="27">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="O67" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P67" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R67" s="27">
+      <c r="X67" s="21">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="Z67" s="27">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="AA67" s="28">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="S67" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="T67" s="21">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="V67" s="27">
-        <f t="shared" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="W67" s="28">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="X67" s="21">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="Z67" s="27">
-        <f t="shared" si="62"/>
-        <v>0</v>
-      </c>
-      <c r="AA67" s="28">
-        <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
       <c r="AB67" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30602,7 +30614,7 @@
       <c r="C68" s="32"/>
       <c r="D68" s="33"/>
       <c r="F68" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G68" s="28">
@@ -30610,67 +30622,67 @@
         <v>0</v>
       </c>
       <c r="H68" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="J68" s="27">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="K68" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L68" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="N68" s="27">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="O68" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P68" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R68" s="27">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="S68" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="J68" s="27">
+      <c r="T68" s="21">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="V68" s="27">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="W68" s="28">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="K68" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L68" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="N68" s="27">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="O68" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P68" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R68" s="27">
+      <c r="X68" s="21">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="Z68" s="27">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="AA68" s="28">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="S68" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="T68" s="21">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="V68" s="27">
-        <f t="shared" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="W68" s="28">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="X68" s="21">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="Z68" s="27">
-        <f t="shared" si="62"/>
-        <v>0</v>
-      </c>
-      <c r="AA68" s="28">
-        <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
       <c r="AB68" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30688,7 +30700,7 @@
         <v>7.8118999999999994E-2</v>
       </c>
       <c r="F69" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>7.0307099999999997E-2</v>
       </c>
       <c r="G69" s="28">
@@ -30696,82 +30708,82 @@
         <v>7.0307099999999997E-2</v>
       </c>
       <c r="H69" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>7.0307099999999997E-2</v>
       </c>
       <c r="I69" s="26">
         <v>0</v>
       </c>
       <c r="J69" s="27">
-        <f t="shared" si="58"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="K69" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L69" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="M69" s="26">
         <v>0</v>
       </c>
       <c r="N69" s="27">
-        <f t="shared" si="59"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="O69" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P69" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q69" s="26">
         <v>8.1810999999999995E-2</v>
       </c>
       <c r="R69" s="27">
-        <f t="shared" si="60"/>
+        <f t="shared" si="66"/>
         <v>7.3629899999999998E-2</v>
       </c>
       <c r="S69" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>7.3629899999999998E-2</v>
       </c>
       <c r="T69" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>7.3629899999999998E-2</v>
       </c>
       <c r="U69" s="26">
         <v>0.13589300000000001</v>
       </c>
       <c r="V69" s="27">
-        <f t="shared" si="61"/>
+        <f t="shared" si="67"/>
         <v>0.12230370000000002</v>
       </c>
       <c r="W69" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.12230370000000002</v>
       </c>
       <c r="X69" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0.12230370000000002</v>
       </c>
       <c r="Y69" s="26">
         <v>0</v>
       </c>
       <c r="Z69" s="27">
-        <f t="shared" si="62"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="AA69" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB69" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30789,7 +30801,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G70" s="28">
@@ -30797,82 +30809,82 @@
         <v>0</v>
       </c>
       <c r="H70" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="I70" s="26">
+        <v>0</v>
+      </c>
+      <c r="J70" s="27">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="K70" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L70" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="M70" s="26">
+        <v>0</v>
+      </c>
+      <c r="N70" s="27">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="O70" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P70" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Q70" s="26">
+        <v>0</v>
+      </c>
+      <c r="R70" s="27">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="S70" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="I70" s="26">
-        <v>0</v>
-      </c>
-      <c r="J70" s="27">
+      <c r="T70" s="21">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="U70" s="26">
+        <v>0</v>
+      </c>
+      <c r="V70" s="27">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="W70" s="28">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="K70" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L70" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="M70" s="26">
-        <v>0</v>
-      </c>
-      <c r="N70" s="27">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="O70" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P70" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="Q70" s="26">
-        <v>0</v>
-      </c>
-      <c r="R70" s="27">
+      <c r="X70" s="21">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="Y70" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="27">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="AA70" s="28">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="S70" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="T70" s="21">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="U70" s="26">
-        <v>0</v>
-      </c>
-      <c r="V70" s="27">
-        <f t="shared" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="W70" s="28">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="X70" s="21">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="Y70" s="26">
-        <v>0</v>
-      </c>
-      <c r="Z70" s="27">
-        <f t="shared" si="62"/>
-        <v>0</v>
-      </c>
-      <c r="AA70" s="28">
-        <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
       <c r="AB70" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30890,7 +30902,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="27">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="G71" s="28">
@@ -30898,82 +30910,82 @@
         <v>0</v>
       </c>
       <c r="H71" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="I71" s="26">
+        <v>0</v>
+      </c>
+      <c r="J71" s="27">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="K71" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L71" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="M71" s="26">
+        <v>0</v>
+      </c>
+      <c r="N71" s="27">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="O71" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P71" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Q71" s="26">
+        <v>0</v>
+      </c>
+      <c r="R71" s="27">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="S71" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="I71" s="26">
-        <v>0</v>
-      </c>
-      <c r="J71" s="27">
+      <c r="T71" s="21">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="U71" s="26">
+        <v>0</v>
+      </c>
+      <c r="V71" s="27">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="W71" s="28">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="K71" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L71" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="M71" s="26">
-        <v>0</v>
-      </c>
-      <c r="N71" s="27">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="O71" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P71" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="Q71" s="26">
-        <v>0</v>
-      </c>
-      <c r="R71" s="27">
+      <c r="X71" s="21">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="Y71" s="26">
+        <v>0</v>
+      </c>
+      <c r="Z71" s="27">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="AA71" s="28">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="S71" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="T71" s="21">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="U71" s="26">
-        <v>0</v>
-      </c>
-      <c r="V71" s="27">
-        <f t="shared" si="61"/>
-        <v>0</v>
-      </c>
-      <c r="W71" s="28">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="X71" s="21">
-        <f t="shared" si="54"/>
-        <v>0</v>
-      </c>
-      <c r="Y71" s="26">
-        <v>0</v>
-      </c>
-      <c r="Z71" s="27">
-        <f t="shared" si="62"/>
-        <v>0</v>
-      </c>
-      <c r="AA71" s="28">
-        <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
       <c r="AB71" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -30986,7 +30998,7 @@
       <c r="C72" s="32"/>
       <c r="D72" s="33"/>
       <c r="F72" s="27">
-        <f t="shared" ref="F72:F78" si="63">E72</f>
+        <f t="shared" ref="F72:F78" si="69">E72</f>
         <v>0</v>
       </c>
       <c r="G72" s="28">
@@ -30994,70 +31006,70 @@
         <v>0</v>
       </c>
       <c r="H72" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="J72" s="27">
+        <f t="shared" ref="J72:J78" si="70">I72</f>
+        <v>0</v>
+      </c>
+      <c r="K72" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L72" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="N72" s="27">
+        <f t="shared" ref="N72:N78" si="71">M72</f>
+        <v>0</v>
+      </c>
+      <c r="O72" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P72" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R72" s="27">
+        <f t="shared" ref="R72:R78" si="72">Q72</f>
+        <v>0</v>
+      </c>
+      <c r="S72" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="J72" s="27">
-        <f t="shared" ref="J72:J78" si="64">I72</f>
-        <v>0</v>
-      </c>
-      <c r="K72" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L72" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="N72" s="27">
-        <f t="shared" ref="N72:N78" si="65">M72</f>
-        <v>0</v>
-      </c>
-      <c r="O72" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P72" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R72" s="27">
-        <f t="shared" ref="R72:R78" si="66">Q72</f>
-        <v>0</v>
-      </c>
-      <c r="S72" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
       <c r="T72" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="U72" s="26">
         <v>90</v>
       </c>
       <c r="V72" s="27">
-        <f t="shared" ref="V72:V78" si="67">U72</f>
+        <f t="shared" ref="V72:V78" si="73">U72</f>
         <v>90</v>
       </c>
       <c r="W72" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>90</v>
       </c>
       <c r="X72" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>90</v>
       </c>
       <c r="Z72" s="27">
-        <f t="shared" ref="Z72:Z78" si="68">Y72</f>
+        <f t="shared" ref="Z72:Z78" si="74">Y72</f>
         <v>0</v>
       </c>
       <c r="AA72" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB72" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -31070,7 +31082,7 @@
       <c r="C73" s="32"/>
       <c r="D73" s="33"/>
       <c r="F73" s="27">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="G73" s="28">
@@ -31078,70 +31090,70 @@
         <v>0</v>
       </c>
       <c r="H73" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="I73" s="26">
         <v>100</v>
       </c>
       <c r="J73" s="27">
-        <f t="shared" si="64"/>
+        <f t="shared" si="70"/>
         <v>100</v>
       </c>
       <c r="K73" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>100</v>
       </c>
       <c r="L73" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>100</v>
       </c>
       <c r="N73" s="27">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="O73" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P73" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="R73" s="27">
-        <f t="shared" si="66"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="S73" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="T73" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V73" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="W73" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X73" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Z73" s="27">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="AA73" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB73" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -31154,7 +31166,7 @@
       <c r="C74" s="32"/>
       <c r="D74" s="33"/>
       <c r="F74" s="27">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="G74" s="28">
@@ -31162,70 +31174,70 @@
         <v>0</v>
       </c>
       <c r="H74" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="J74" s="27">
-        <f t="shared" si="64"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="K74" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L74" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="M74" s="26">
         <v>100</v>
       </c>
       <c r="N74" s="27">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>100</v>
       </c>
       <c r="O74" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>100</v>
       </c>
       <c r="P74" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>100</v>
       </c>
       <c r="R74" s="27">
-        <f t="shared" si="66"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="S74" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="T74" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V74" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="W74" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X74" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Z74" s="27">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="AA74" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB74" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -31241,7 +31253,7 @@
         <v>50</v>
       </c>
       <c r="F75" s="27">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>50</v>
       </c>
       <c r="G75" s="28">
@@ -31249,73 +31261,73 @@
         <v>50</v>
       </c>
       <c r="H75" s="21">
+        <f t="shared" si="62"/>
+        <v>50</v>
+      </c>
+      <c r="J75" s="27">
+        <f t="shared" si="70"/>
+        <v>0</v>
+      </c>
+      <c r="K75" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L75" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="N75" s="27">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="O75" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P75" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R75" s="27">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="S75" s="28">
         <f t="shared" si="56"/>
-        <v>50</v>
-      </c>
-      <c r="J75" s="27">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="K75" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L75" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="N75" s="27">
-        <f t="shared" si="65"/>
-        <v>0</v>
-      </c>
-      <c r="O75" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P75" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R75" s="27">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="S75" s="28">
-        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="T75" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="U75" s="26">
         <v>10</v>
       </c>
       <c r="V75" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>10</v>
       </c>
       <c r="W75" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>10</v>
       </c>
       <c r="X75" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>10</v>
       </c>
       <c r="Y75" s="26">
         <v>40</v>
       </c>
       <c r="Z75" s="27">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>40</v>
       </c>
       <c r="AA75" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>40</v>
       </c>
       <c r="AB75" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>40</v>
       </c>
     </row>
@@ -31331,7 +31343,7 @@
         <v>50</v>
       </c>
       <c r="F76" s="27">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>50</v>
       </c>
       <c r="G76" s="28">
@@ -31339,70 +31351,70 @@
         <v>50</v>
       </c>
       <c r="H76" s="21">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>50</v>
       </c>
       <c r="J76" s="27">
-        <f t="shared" si="64"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="K76" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L76" s="21">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N76" s="27">
-        <f t="shared" si="65"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="O76" s="28">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P76" s="21">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q76" s="26">
         <v>100</v>
       </c>
       <c r="R76" s="27">
-        <f t="shared" si="66"/>
+        <f t="shared" si="72"/>
         <v>100</v>
       </c>
       <c r="S76" s="28">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>100</v>
       </c>
       <c r="T76" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>100</v>
       </c>
       <c r="V76" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="W76" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X76" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Z76" s="27">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="AA76" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB76" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -31415,7 +31427,7 @@
       <c r="C77" s="32"/>
       <c r="D77" s="33"/>
       <c r="F77" s="27">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="G77" s="28">
@@ -31423,70 +31435,70 @@
         <v>0</v>
       </c>
       <c r="H77" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="J77" s="27">
+        <f t="shared" si="70"/>
+        <v>0</v>
+      </c>
+      <c r="K77" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L77" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="N77" s="27">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="O77" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P77" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R77" s="27">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="S77" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="J77" s="27">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="K77" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L77" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="N77" s="27">
-        <f t="shared" si="65"/>
-        <v>0</v>
-      </c>
-      <c r="O77" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P77" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R77" s="27">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="S77" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
       <c r="T77" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V77" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="W77" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X77" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Y77" s="26">
         <v>60</v>
       </c>
       <c r="Z77" s="27">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>60</v>
       </c>
       <c r="AA77" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>60</v>
       </c>
       <c r="AB77" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>60</v>
       </c>
     </row>
@@ -31499,7 +31511,7 @@
       <c r="C78" s="32"/>
       <c r="D78" s="33"/>
       <c r="F78" s="27">
-        <f t="shared" si="63"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="G78" s="28">
@@ -31507,67 +31519,67 @@
         <v>0</v>
       </c>
       <c r="H78" s="21">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="J78" s="27">
+        <f t="shared" si="70"/>
+        <v>0</v>
+      </c>
+      <c r="K78" s="28">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="L78" s="21">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="N78" s="27">
+        <f t="shared" si="71"/>
+        <v>0</v>
+      </c>
+      <c r="O78" s="28">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="P78" s="21">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="R78" s="27">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="S78" s="28">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="J78" s="27">
-        <f t="shared" si="64"/>
-        <v>0</v>
-      </c>
-      <c r="K78" s="28">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="L78" s="21">
-        <f t="shared" si="51"/>
-        <v>0</v>
-      </c>
-      <c r="N78" s="27">
-        <f t="shared" si="65"/>
-        <v>0</v>
-      </c>
-      <c r="O78" s="28">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="P78" s="21">
-        <f t="shared" si="52"/>
-        <v>0</v>
-      </c>
-      <c r="R78" s="27">
-        <f t="shared" si="66"/>
-        <v>0</v>
-      </c>
-      <c r="S78" s="28">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
       <c r="T78" s="21">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V78" s="27">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="W78" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="X78" s="21">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Z78" s="27">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="AA78" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="AB78" s="21">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
@@ -31580,86 +31592,86 @@
         <v>0.05</v>
       </c>
       <c r="C79" s="36">
-        <f t="shared" ref="C79:C84" si="69">(1/0.05) * 0.5</f>
+        <f t="shared" ref="C79:C84" si="75">(1/0.05) * 0.5</f>
         <v>10</v>
       </c>
       <c r="D79" s="33">
-        <f t="shared" ref="D79:D84" si="70">(1/0.05) * 0.75</f>
+        <f t="shared" ref="D79:D84" si="76">(1/0.05) * 0.75</f>
         <v>15</v>
       </c>
       <c r="F79" s="27">
-        <f t="shared" ref="F79:F94" si="71">$B79*E79</f>
+        <f t="shared" ref="F79:F94" si="77">$B79*E79</f>
         <v>0</v>
       </c>
       <c r="G79" s="28">
-        <f t="shared" ref="G79:G84" si="72">$C79*F79</f>
+        <f t="shared" ref="G79:G84" si="78">$C79*F79</f>
         <v>0</v>
       </c>
       <c r="H79" s="35">
-        <f t="shared" ref="H79:H84" si="73">$D79*G79</f>
+        <f t="shared" ref="H79:H84" si="79">$D79*G79</f>
         <v>0</v>
       </c>
       <c r="J79" s="27">
-        <f t="shared" ref="J79:J94" si="74">$B79*I79</f>
+        <f t="shared" ref="J79:J94" si="80">$B79*I79</f>
         <v>0</v>
       </c>
       <c r="K79" s="28">
-        <f t="shared" ref="K79:K84" si="75">$C79*J79</f>
+        <f t="shared" ref="K79:K84" si="81">$C79*J79</f>
         <v>0</v>
       </c>
       <c r="L79" s="35">
-        <f t="shared" ref="L79:L84" si="76">$D79*K79</f>
+        <f t="shared" ref="L79:L84" si="82">$D79*K79</f>
         <v>0</v>
       </c>
       <c r="N79" s="27">
-        <f t="shared" ref="N79:N94" si="77">$B79*M79</f>
+        <f t="shared" ref="N79:N94" si="83">$B79*M79</f>
         <v>0</v>
       </c>
       <c r="O79" s="28">
-        <f t="shared" ref="O79:O84" si="78">$C79*N79</f>
+        <f t="shared" ref="O79:O84" si="84">$C79*N79</f>
         <v>0</v>
       </c>
       <c r="P79" s="35">
-        <f t="shared" ref="P79:P84" si="79">$D79*O79</f>
+        <f t="shared" ref="P79:P84" si="85">$D79*O79</f>
         <v>0</v>
       </c>
       <c r="Q79" s="26">
         <v>2</v>
       </c>
       <c r="R79" s="27">
-        <f t="shared" ref="R79:R94" si="80">$B79*Q79</f>
+        <f t="shared" ref="R79:R94" si="86">$B79*Q79</f>
         <v>0.1</v>
       </c>
       <c r="S79" s="28">
-        <f t="shared" ref="S79:S84" si="81">$C79*R79</f>
+        <f t="shared" ref="S79:S84" si="87">$C79*R79</f>
         <v>1</v>
       </c>
       <c r="T79" s="35">
-        <f t="shared" ref="T79:T84" si="82">$D79*S79</f>
+        <f t="shared" ref="T79:T84" si="88">$D79*S79</f>
         <v>15</v>
       </c>
       <c r="V79" s="27">
-        <f t="shared" ref="V79:V94" si="83">$B79*U79</f>
+        <f t="shared" ref="V79:V94" si="89">$B79*U79</f>
         <v>0</v>
       </c>
       <c r="W79" s="28">
-        <f t="shared" ref="W79:W84" si="84">$C79*V79</f>
+        <f t="shared" ref="W79:W84" si="90">$C79*V79</f>
         <v>0</v>
       </c>
       <c r="X79" s="35">
-        <f t="shared" ref="X79:X84" si="85">$D79*W79</f>
+        <f t="shared" ref="X79:X84" si="91">$D79*W79</f>
         <v>0</v>
       </c>
       <c r="Z79" s="27">
-        <f t="shared" ref="Z79:Z94" si="86">$B79*Y79</f>
+        <f t="shared" ref="Z79:Z94" si="92">$B79*Y79</f>
         <v>0</v>
       </c>
       <c r="AA79" s="28">
-        <f t="shared" ref="AA79:AA84" si="87">$C79*Z79</f>
+        <f t="shared" ref="AA79:AA84" si="93">$C79*Z79</f>
         <v>0</v>
       </c>
       <c r="AB79" s="35">
-        <f t="shared" ref="AB79:AB84" si="88">$D79*AA79</f>
+        <f t="shared" ref="AB79:AB84" si="94">$D79*AA79</f>
         <v>0</v>
       </c>
     </row>
@@ -31672,86 +31684,86 @@
         <v>0.05</v>
       </c>
       <c r="C80" s="36">
-        <f t="shared" si="69"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="D80" s="33">
-        <f t="shared" si="70"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="F80" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G80" s="28">
-        <f t="shared" si="72"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H80" s="35">
-        <f t="shared" si="73"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="J80" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="K80" s="28">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="L80" s="35">
-        <f t="shared" si="76"/>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="N80" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O80" s="28">
-        <f t="shared" si="78"/>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="P80" s="35">
-        <f t="shared" si="79"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="Q80" s="26">
         <v>5</v>
       </c>
       <c r="R80" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.25</v>
       </c>
       <c r="S80" s="28">
-        <f t="shared" si="81"/>
+        <f t="shared" si="87"/>
         <v>2.5</v>
       </c>
       <c r="T80" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>37.5</v>
       </c>
       <c r="V80" s="27">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="W80" s="28">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="X80" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="Z80" s="27">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AA80" s="28">
-        <f t="shared" si="87"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AB80" s="35">
-        <f t="shared" si="88"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
     </row>
@@ -31764,101 +31776,101 @@
         <v>0.05</v>
       </c>
       <c r="C81" s="36">
-        <f t="shared" si="69"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="D81" s="33">
-        <f t="shared" si="70"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="E81" s="26">
         <v>0.2</v>
       </c>
       <c r="F81" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="G81" s="28">
-        <f t="shared" si="72"/>
+        <f t="shared" si="78"/>
         <v>0.10000000000000002</v>
       </c>
       <c r="H81" s="35">
-        <f t="shared" si="73"/>
+        <f t="shared" si="79"/>
         <v>1.5000000000000002</v>
       </c>
       <c r="I81" s="26">
         <v>1</v>
       </c>
       <c r="J81" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0.05</v>
       </c>
       <c r="K81" s="28">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>0.5</v>
       </c>
       <c r="L81" s="35">
-        <f t="shared" si="76"/>
+        <f t="shared" si="82"/>
         <v>7.5</v>
       </c>
       <c r="M81" s="26">
         <v>2.5</v>
       </c>
       <c r="N81" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0.125</v>
       </c>
       <c r="O81" s="28">
-        <f t="shared" si="78"/>
+        <f t="shared" si="84"/>
         <v>1.25</v>
       </c>
       <c r="P81" s="35">
-        <f t="shared" si="79"/>
+        <f t="shared" si="85"/>
         <v>18.75</v>
       </c>
       <c r="Q81" s="26">
         <v>1</v>
       </c>
       <c r="R81" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.05</v>
       </c>
       <c r="S81" s="28">
-        <f t="shared" si="81"/>
+        <f t="shared" si="87"/>
         <v>0.5</v>
       </c>
       <c r="T81" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>7.5</v>
       </c>
       <c r="U81" s="26">
         <v>1.5</v>
       </c>
       <c r="V81" s="27">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="W81" s="28">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0.75000000000000011</v>
       </c>
       <c r="X81" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>11.250000000000002</v>
       </c>
       <c r="Y81" s="26">
         <v>2</v>
       </c>
       <c r="Z81" s="27">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>0.1</v>
       </c>
       <c r="AA81" s="28">
-        <f t="shared" si="87"/>
+        <f t="shared" si="93"/>
         <v>1</v>
       </c>
       <c r="AB81" s="35">
-        <f t="shared" si="88"/>
+        <f t="shared" si="94"/>
         <v>15</v>
       </c>
     </row>
@@ -31871,101 +31883,101 @@
         <v>0.05</v>
       </c>
       <c r="C82" s="36">
-        <f t="shared" si="69"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="D82" s="33">
-        <f t="shared" si="70"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="E82" s="26">
         <v>70</v>
       </c>
       <c r="F82" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>3.5</v>
       </c>
       <c r="G82" s="28">
-        <f t="shared" si="72"/>
+        <f t="shared" si="78"/>
         <v>35</v>
       </c>
       <c r="H82" s="35">
-        <f t="shared" si="73"/>
+        <f t="shared" si="79"/>
         <v>525</v>
       </c>
       <c r="I82" s="26">
         <v>60</v>
       </c>
       <c r="J82" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>3</v>
       </c>
       <c r="K82" s="28">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>30</v>
       </c>
       <c r="L82" s="35">
-        <f t="shared" si="76"/>
+        <f t="shared" si="82"/>
         <v>450</v>
       </c>
       <c r="M82" s="26">
         <v>5</v>
       </c>
       <c r="N82" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0.25</v>
       </c>
       <c r="O82" s="28">
-        <f t="shared" si="78"/>
+        <f t="shared" si="84"/>
         <v>2.5</v>
       </c>
       <c r="P82" s="35">
-        <f t="shared" si="79"/>
+        <f t="shared" si="85"/>
         <v>37.5</v>
       </c>
       <c r="Q82" s="26">
         <v>15</v>
       </c>
       <c r="R82" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.75</v>
       </c>
       <c r="S82" s="28">
-        <f t="shared" si="81"/>
+        <f t="shared" si="87"/>
         <v>7.5</v>
       </c>
       <c r="T82" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>112.5</v>
       </c>
       <c r="U82" s="26">
         <v>90</v>
       </c>
       <c r="V82" s="27">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>4.5</v>
       </c>
       <c r="W82" s="28">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>45</v>
       </c>
       <c r="X82" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>675</v>
       </c>
       <c r="Y82" s="26">
         <v>70</v>
       </c>
       <c r="Z82" s="27">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>3.5</v>
       </c>
       <c r="AA82" s="28">
-        <f t="shared" si="87"/>
+        <f t="shared" si="93"/>
         <v>35</v>
       </c>
       <c r="AB82" s="35">
-        <f t="shared" si="88"/>
+        <f t="shared" si="94"/>
         <v>525</v>
       </c>
     </row>
@@ -31978,89 +31990,89 @@
         <v>0.05</v>
       </c>
       <c r="C83" s="36">
-        <f t="shared" si="69"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="D83" s="33">
-        <f t="shared" si="70"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="F83" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G83" s="28">
-        <f t="shared" si="72"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H83" s="35">
-        <f t="shared" si="73"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="J83" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="K83" s="28">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="L83" s="35">
-        <f t="shared" si="76"/>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="N83" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O83" s="28">
-        <f t="shared" si="78"/>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="P83" s="35">
-        <f t="shared" si="79"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="Q83" s="26">
         <v>2.5</v>
       </c>
       <c r="R83" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.125</v>
       </c>
       <c r="S83" s="28">
-        <f t="shared" si="81"/>
+        <f t="shared" si="87"/>
         <v>1.25</v>
       </c>
       <c r="T83" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>18.75</v>
       </c>
       <c r="U83" s="26">
         <v>1</v>
       </c>
       <c r="V83" s="27">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0.05</v>
       </c>
       <c r="W83" s="28">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0.5</v>
       </c>
       <c r="X83" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>7.5</v>
       </c>
       <c r="Z83" s="27">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AA83" s="28">
-        <f t="shared" si="87"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AB83" s="35">
-        <f t="shared" si="88"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
     </row>
@@ -32073,89 +32085,89 @@
         <v>0.05</v>
       </c>
       <c r="C84" s="36">
-        <f t="shared" si="69"/>
+        <f t="shared" si="75"/>
         <v>10</v>
       </c>
       <c r="D84" s="33">
-        <f t="shared" si="70"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="F84" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G84" s="28">
-        <f t="shared" si="72"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H84" s="35">
-        <f t="shared" si="73"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="J84" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="K84" s="28">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="L84" s="35">
-        <f t="shared" si="76"/>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="N84" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O84" s="28">
-        <f t="shared" si="78"/>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="P84" s="35">
-        <f t="shared" si="79"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="Q84" s="26">
         <v>80</v>
       </c>
       <c r="R84" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>4</v>
       </c>
       <c r="S84" s="28">
-        <f t="shared" si="81"/>
+        <f t="shared" si="87"/>
         <v>40</v>
       </c>
       <c r="T84" s="35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>600</v>
       </c>
       <c r="U84" s="26">
         <v>5</v>
       </c>
       <c r="V84" s="27">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0.25</v>
       </c>
       <c r="W84" s="28">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>2.5</v>
       </c>
       <c r="X84" s="35">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>37.5</v>
       </c>
       <c r="Z84" s="27">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AA84" s="28">
-        <f t="shared" si="87"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="AB84" s="35">
-        <f t="shared" si="88"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
     </row>
@@ -32170,81 +32182,81 @@
       <c r="C85" s="32"/>
       <c r="D85" s="33"/>
       <c r="F85" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G85" s="28">
-        <f t="shared" ref="G85:H94" si="89">F85</f>
+        <f t="shared" ref="G85:H94" si="95">F85</f>
         <v>0</v>
       </c>
       <c r="H85" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="I85" s="26">
         <v>0.2</v>
       </c>
       <c r="J85" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="K85" s="28">
-        <f t="shared" ref="K85:L94" si="90">J85</f>
+        <f t="shared" ref="K85:L94" si="96">J85</f>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="L85" s="35">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="N85" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O85" s="28">
-        <f t="shared" ref="O85:P94" si="91">N85</f>
+        <f t="shared" ref="O85:P94" si="97">N85</f>
         <v>0</v>
       </c>
       <c r="P85" s="35">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="Q85" s="26">
         <v>2</v>
       </c>
       <c r="R85" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.1</v>
       </c>
       <c r="S85" s="28">
-        <f t="shared" ref="S85:T94" si="92">R85</f>
+        <f t="shared" ref="S85:T94" si="98">R85</f>
         <v>0.1</v>
       </c>
       <c r="T85" s="35">
+        <f t="shared" si="98"/>
+        <v>0.1</v>
+      </c>
+      <c r="V85" s="27">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="W85" s="28">
+        <f t="shared" ref="W85:X94" si="99">V85</f>
+        <v>0</v>
+      </c>
+      <c r="X85" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z85" s="27">
         <f t="shared" si="92"/>
-        <v>0.1</v>
-      </c>
-      <c r="V85" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W85" s="28">
-        <f t="shared" ref="W85:X94" si="93">V85</f>
-        <v>0</v>
-      </c>
-      <c r="X85" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z85" s="27">
-        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="AA85" s="28">
-        <f t="shared" ref="AA85:AB94" si="94">Z85</f>
+        <f t="shared" ref="AA85:AB94" si="100">Z85</f>
         <v>0</v>
       </c>
       <c r="AB85" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
@@ -32259,81 +32271,81 @@
       <c r="C86" s="32"/>
       <c r="D86" s="33"/>
       <c r="F86" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G86" s="28">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="H86" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="I86" s="26">
         <v>60</v>
       </c>
       <c r="J86" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>3</v>
       </c>
       <c r="K86" s="28">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>3</v>
       </c>
       <c r="L86" s="35">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>3</v>
       </c>
       <c r="N86" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O86" s="28">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="P86" s="35">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="Q86" s="26">
         <v>90</v>
       </c>
       <c r="R86" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>4.5</v>
       </c>
       <c r="S86" s="28">
+        <f t="shared" si="98"/>
+        <v>4.5</v>
+      </c>
+      <c r="T86" s="35">
+        <f t="shared" si="98"/>
+        <v>4.5</v>
+      </c>
+      <c r="V86" s="27">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="W86" s="28">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X86" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z86" s="27">
         <f t="shared" si="92"/>
-        <v>4.5</v>
-      </c>
-      <c r="T86" s="35">
-        <f t="shared" si="92"/>
-        <v>4.5</v>
-      </c>
-      <c r="V86" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W86" s="28">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="X86" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z86" s="27">
-        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="AA86" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AB86" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
@@ -32351,90 +32363,90 @@
         <v>0.5</v>
       </c>
       <c r="F87" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G87" s="28">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H87" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I87" s="26">
         <v>0.4</v>
       </c>
       <c r="J87" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="K87" s="28">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="L87" s="35">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="M87" s="26">
         <v>0.2</v>
       </c>
       <c r="N87" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="O87" s="28">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="P87" s="35">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="Q87" s="26">
         <v>4</v>
       </c>
       <c r="R87" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.2</v>
       </c>
       <c r="S87" s="28">
-        <f t="shared" si="92"/>
+        <f t="shared" si="98"/>
         <v>0.2</v>
       </c>
       <c r="T87" s="35">
-        <f t="shared" si="92"/>
+        <f t="shared" si="98"/>
         <v>0.2</v>
       </c>
       <c r="U87" s="26">
         <v>1</v>
       </c>
       <c r="V87" s="27">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0.05</v>
       </c>
       <c r="W87" s="28">
-        <f t="shared" si="93"/>
+        <f t="shared" si="99"/>
         <v>0.05</v>
       </c>
       <c r="X87" s="35">
-        <f t="shared" si="93"/>
+        <f t="shared" si="99"/>
         <v>0.05</v>
       </c>
       <c r="Y87" s="26">
         <v>1.5</v>
       </c>
       <c r="Z87" s="27">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="AA87" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="AB87" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>7.5000000000000011E-2</v>
       </c>
     </row>
@@ -32452,90 +32464,90 @@
         <v>70</v>
       </c>
       <c r="F88" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>3.5</v>
       </c>
       <c r="G88" s="28">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>3.5</v>
       </c>
       <c r="H88" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>3.5</v>
       </c>
       <c r="I88" s="26">
         <v>60</v>
       </c>
       <c r="J88" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>3</v>
       </c>
       <c r="K88" s="28">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>3</v>
       </c>
       <c r="L88" s="35">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>3</v>
       </c>
       <c r="M88" s="26">
         <v>70</v>
       </c>
       <c r="N88" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>3.5</v>
       </c>
       <c r="O88" s="28">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>3.5</v>
       </c>
       <c r="P88" s="35">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>3.5</v>
       </c>
       <c r="Q88" s="26">
         <v>100</v>
       </c>
       <c r="R88" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>5</v>
       </c>
       <c r="S88" s="28">
-        <f t="shared" si="92"/>
+        <f t="shared" si="98"/>
         <v>5</v>
       </c>
       <c r="T88" s="35">
-        <f t="shared" si="92"/>
+        <f t="shared" si="98"/>
         <v>5</v>
       </c>
       <c r="U88" s="26">
         <v>90</v>
       </c>
       <c r="V88" s="27">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>4.5</v>
       </c>
       <c r="W88" s="28">
-        <f t="shared" si="93"/>
+        <f t="shared" si="99"/>
         <v>4.5</v>
       </c>
       <c r="X88" s="35">
-        <f t="shared" si="93"/>
+        <f t="shared" si="99"/>
         <v>4.5</v>
       </c>
       <c r="Y88" s="26">
         <v>70</v>
       </c>
       <c r="Z88" s="27">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>3.5</v>
       </c>
       <c r="AA88" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>3.5</v>
       </c>
       <c r="AB88" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>3.5</v>
       </c>
     </row>
@@ -32550,75 +32562,75 @@
       <c r="C89" s="32"/>
       <c r="D89" s="33"/>
       <c r="F89" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G89" s="28">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="H89" s="35">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="J89" s="27">
+        <f t="shared" si="80"/>
+        <v>0</v>
+      </c>
+      <c r="K89" s="28">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="L89" s="35">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="N89" s="27">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="O89" s="28">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="P89" s="35">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="R89" s="27">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+      <c r="S89" s="28">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="T89" s="35">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="V89" s="27">
         <f t="shared" si="89"/>
         <v>0</v>
       </c>
-      <c r="H89" s="35">
-        <f t="shared" si="89"/>
-        <v>0</v>
-      </c>
-      <c r="J89" s="27">
-        <f t="shared" si="74"/>
-        <v>0</v>
-      </c>
-      <c r="K89" s="28">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
-      <c r="L89" s="35">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
-      <c r="N89" s="27">
-        <f t="shared" si="77"/>
-        <v>0</v>
-      </c>
-      <c r="O89" s="28">
-        <f t="shared" si="91"/>
-        <v>0</v>
-      </c>
-      <c r="P89" s="35">
-        <f t="shared" si="91"/>
-        <v>0</v>
-      </c>
-      <c r="R89" s="27">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="S89" s="28">
+      <c r="W89" s="28">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X89" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z89" s="27">
         <f t="shared" si="92"/>
         <v>0</v>
       </c>
-      <c r="T89" s="35">
-        <f t="shared" si="92"/>
-        <v>0</v>
-      </c>
-      <c r="V89" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W89" s="28">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="X89" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z89" s="27">
-        <f t="shared" si="86"/>
-        <v>0</v>
-      </c>
       <c r="AA89" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AB89" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
@@ -32633,75 +32645,75 @@
       <c r="C90" s="32"/>
       <c r="D90" s="33"/>
       <c r="F90" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G90" s="28">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="H90" s="35">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="J90" s="27">
+        <f t="shared" si="80"/>
+        <v>0</v>
+      </c>
+      <c r="K90" s="28">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="L90" s="35">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="N90" s="27">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="O90" s="28">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="P90" s="35">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="R90" s="27">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+      <c r="S90" s="28">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="T90" s="35">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="V90" s="27">
         <f t="shared" si="89"/>
         <v>0</v>
       </c>
-      <c r="H90" s="35">
-        <f t="shared" si="89"/>
-        <v>0</v>
-      </c>
-      <c r="J90" s="27">
-        <f t="shared" si="74"/>
-        <v>0</v>
-      </c>
-      <c r="K90" s="28">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
-      <c r="L90" s="35">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
-      <c r="N90" s="27">
-        <f t="shared" si="77"/>
-        <v>0</v>
-      </c>
-      <c r="O90" s="28">
-        <f t="shared" si="91"/>
-        <v>0</v>
-      </c>
-      <c r="P90" s="35">
-        <f t="shared" si="91"/>
-        <v>0</v>
-      </c>
-      <c r="R90" s="27">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="S90" s="28">
+      <c r="W90" s="28">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X90" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z90" s="27">
         <f t="shared" si="92"/>
         <v>0</v>
       </c>
-      <c r="T90" s="35">
-        <f t="shared" si="92"/>
-        <v>0</v>
-      </c>
-      <c r="V90" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W90" s="28">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="X90" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z90" s="27">
-        <f t="shared" si="86"/>
-        <v>0</v>
-      </c>
       <c r="AA90" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AB90" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
@@ -32716,75 +32728,75 @@
       <c r="C91" s="32"/>
       <c r="D91" s="33"/>
       <c r="F91" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G91" s="28">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="H91" s="35">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="J91" s="27">
+        <f t="shared" si="80"/>
+        <v>0</v>
+      </c>
+      <c r="K91" s="28">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="L91" s="35">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="N91" s="27">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="O91" s="28">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="P91" s="35">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="R91" s="27">
+        <f t="shared" si="86"/>
+        <v>0</v>
+      </c>
+      <c r="S91" s="28">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="T91" s="35">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="V91" s="27">
         <f t="shared" si="89"/>
         <v>0</v>
       </c>
-      <c r="H91" s="35">
-        <f t="shared" si="89"/>
-        <v>0</v>
-      </c>
-      <c r="J91" s="27">
-        <f t="shared" si="74"/>
-        <v>0</v>
-      </c>
-      <c r="K91" s="28">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
-      <c r="L91" s="35">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
-      <c r="N91" s="27">
-        <f t="shared" si="77"/>
-        <v>0</v>
-      </c>
-      <c r="O91" s="28">
-        <f t="shared" si="91"/>
-        <v>0</v>
-      </c>
-      <c r="P91" s="35">
-        <f t="shared" si="91"/>
-        <v>0</v>
-      </c>
-      <c r="R91" s="27">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="S91" s="28">
+      <c r="W91" s="28">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X91" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z91" s="27">
         <f t="shared" si="92"/>
         <v>0</v>
       </c>
-      <c r="T91" s="35">
-        <f t="shared" si="92"/>
-        <v>0</v>
-      </c>
-      <c r="V91" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W91" s="28">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="X91" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z91" s="27">
-        <f t="shared" si="86"/>
-        <v>0</v>
-      </c>
       <c r="AA91" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AB91" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
@@ -32799,78 +32811,78 @@
       <c r="C92" s="32"/>
       <c r="D92" s="33"/>
       <c r="F92" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G92" s="28">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="H92" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="J92" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="K92" s="28">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="L92" s="35">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="N92" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O92" s="28">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="P92" s="35">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="Q92" s="26">
         <v>18</v>
       </c>
       <c r="R92" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.9</v>
       </c>
       <c r="S92" s="28">
+        <f t="shared" si="98"/>
+        <v>0.9</v>
+      </c>
+      <c r="T92" s="35">
+        <f t="shared" si="98"/>
+        <v>0.9</v>
+      </c>
+      <c r="V92" s="27">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="W92" s="28">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X92" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z92" s="27">
         <f t="shared" si="92"/>
-        <v>0.9</v>
-      </c>
-      <c r="T92" s="35">
-        <f t="shared" si="92"/>
-        <v>0.9</v>
-      </c>
-      <c r="V92" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W92" s="28">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="X92" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z92" s="27">
-        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="AA92" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AB92" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
@@ -32885,78 +32897,78 @@
       <c r="C93" s="32"/>
       <c r="D93" s="33"/>
       <c r="F93" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G93" s="28">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="H93" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="J93" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="K93" s="28">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="L93" s="35">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="N93" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O93" s="28">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="P93" s="35">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="Q93" s="26">
         <v>1</v>
       </c>
       <c r="R93" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.05</v>
       </c>
       <c r="S93" s="28">
+        <f t="shared" si="98"/>
+        <v>0.05</v>
+      </c>
+      <c r="T93" s="35">
+        <f t="shared" si="98"/>
+        <v>0.05</v>
+      </c>
+      <c r="V93" s="27">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="W93" s="28">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X93" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z93" s="27">
         <f t="shared" si="92"/>
-        <v>0.05</v>
-      </c>
-      <c r="T93" s="35">
-        <f t="shared" si="92"/>
-        <v>0.05</v>
-      </c>
-      <c r="V93" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W93" s="28">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="X93" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z93" s="27">
-        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="AA93" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AB93" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
@@ -32971,78 +32983,78 @@
       <c r="C94" s="32"/>
       <c r="D94" s="33"/>
       <c r="F94" s="27">
-        <f t="shared" si="71"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="G94" s="28">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="H94" s="35">
-        <f t="shared" si="89"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="J94" s="27">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="K94" s="28">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="L94" s="35">
-        <f t="shared" si="90"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="N94" s="27">
-        <f t="shared" si="77"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="O94" s="28">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="P94" s="35">
-        <f t="shared" si="91"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="Q94" s="26">
         <v>5</v>
       </c>
       <c r="R94" s="27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="86"/>
         <v>0.25</v>
       </c>
       <c r="S94" s="28">
+        <f t="shared" si="98"/>
+        <v>0.25</v>
+      </c>
+      <c r="T94" s="35">
+        <f t="shared" si="98"/>
+        <v>0.25</v>
+      </c>
+      <c r="V94" s="27">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="W94" s="28">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X94" s="35">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="Z94" s="27">
         <f t="shared" si="92"/>
-        <v>0.25</v>
-      </c>
-      <c r="T94" s="35">
-        <f t="shared" si="92"/>
-        <v>0.25</v>
-      </c>
-      <c r="V94" s="27">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W94" s="28">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="X94" s="35">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="Z94" s="27">
-        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="AA94" s="28">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AB94" s="35">
-        <f t="shared" si="94"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated ground fuel low sev specs
</commit_message>
<xml_diff>
--- a/specifications/ScriptRules_Fire.xlsx
+++ b/specifications/ScriptRules_Fire.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\LFDisturbance\landfiredisturbance\specifications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\landfiredisturbance\specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="313">
   <si>
     <t>Filename</t>
   </si>
@@ -2085,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4074,9 +4074,7 @@
       <c r="B85" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C85" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C85" s="14"/>
       <c r="E85" s="5" t="s">
         <v>96</v>
       </c>
@@ -4091,9 +4089,7 @@
       <c r="B86" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C86" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C86" s="14"/>
       <c r="E86" s="5" t="s">
         <v>96</v>
       </c>
@@ -4108,9 +4104,7 @@
       <c r="B87" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C87" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C87" s="14"/>
       <c r="E87" s="5" t="s">
         <v>96</v>
       </c>
@@ -4125,9 +4119,7 @@
       <c r="B88" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C88" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C88" s="14"/>
       <c r="E88" s="5" t="s">
         <v>96</v>
       </c>
@@ -4142,9 +4134,7 @@
       <c r="B89" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C89" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C89" s="14"/>
       <c r="E89" s="5" t="s">
         <v>96</v>
       </c>
@@ -4159,9 +4149,7 @@
       <c r="B90" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C90" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C90" s="14"/>
       <c r="E90" s="5" t="s">
         <v>96</v>
       </c>
@@ -4176,9 +4164,7 @@
       <c r="B91" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C91" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C91" s="14"/>
       <c r="E91" s="5" t="s">
         <v>96</v>
       </c>
@@ -4193,9 +4179,7 @@
       <c r="B92" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C92" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C92" s="14"/>
       <c r="E92" s="5" t="s">
         <v>96</v>
       </c>
@@ -4210,9 +4194,7 @@
       <c r="B93" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C93" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C93" s="14"/>
       <c r="E93" s="5" t="s">
         <v>96</v>
       </c>
@@ -4227,9 +4209,7 @@
       <c r="B94" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C94" s="14" t="s">
-        <v>216</v>
-      </c>
+      <c r="C94" s="14"/>
       <c r="E94" s="5" t="s">
         <v>96</v>
       </c>

</xml_diff>